<commit_message>
Added all output files and figures
</commit_message>
<xml_diff>
--- a/sensitivityAnalyses/phloemComposition/Phloem_composition.xlsx
+++ b/sensitivityAnalyses/phloemComposition/Phloem_composition.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sanus\Scripts\git\ODE_FBA_Photosynthesis2021\sensitivityAnalyses\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sanus\Scripts\git\ODE_FBA_Photosynthesis2021\sensitivityAnalyses\phloemComposition\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{640F34F6-EF31-4C1D-BA5D-F48786F7DE1A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F4FE5C6-E85A-45FA-B471-5481FE5E3CEB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{C94C3547-597F-4633-AAB4-E9F8CF5D6F73}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{C94C3547-597F-4633-AAB4-E9F8CF5D6F73}"/>
   </bookViews>
   <sheets>
     <sheet name="Phloem_compositions" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="ProcessedWilkinsonDouglas" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -5406,16 +5407,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>1341120</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>550545</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>15240</xdr:rowOff>
+      <xdr:rowOff>34290</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>15240</xdr:colOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>339090</xdr:colOff>
       <xdr:row>42</xdr:row>
-      <xdr:rowOff>68580</xdr:rowOff>
+      <xdr:rowOff>87630</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5746,17 +5747,17 @@
       <selection activeCell="C33" sqref="A1:C33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="14.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="20.5546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.88671875" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="51.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="53.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="28.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="51.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="53.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="28.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A1" s="36" t="s">
         <v>0</v>
       </c>
@@ -5780,7 +5781,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>1</v>
       </c>
@@ -5798,7 +5799,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="16"/>
       <c r="B3" s="17" t="s">
         <v>4</v>
@@ -5814,7 +5815,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="16"/>
       <c r="B4" s="17" t="s">
         <v>5</v>
@@ -5830,7 +5831,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="16"/>
       <c r="B5" s="17" t="s">
         <v>3</v>
@@ -5849,7 +5850,7 @@
         <v>82.666666666666671</v>
       </c>
     </row>
-    <row r="6" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="16"/>
       <c r="B6" s="17" t="s">
         <v>6</v>
@@ -5865,7 +5866,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="16"/>
       <c r="B7" s="17" t="s">
         <v>2</v>
@@ -5881,7 +5882,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="16"/>
       <c r="B8" s="20" t="s">
         <v>37</v>
@@ -5896,7 +5897,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="16"/>
       <c r="B9" s="20" t="s">
         <v>38</v>
@@ -5911,7 +5912,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="16"/>
       <c r="B10" s="20" t="s">
         <v>39</v>
@@ -5926,7 +5927,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>7</v>
       </c>
@@ -5944,7 +5945,7 @@
         <v>4.6222222222222227</v>
       </c>
     </row>
-    <row r="12" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="16"/>
       <c r="B12" s="17" t="s">
         <v>8</v>
@@ -5960,7 +5961,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="16"/>
       <c r="B13" s="17" t="s">
         <v>9</v>
@@ -5976,7 +5977,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="16"/>
       <c r="B14" s="17" t="s">
         <v>10</v>
@@ -5992,7 +5993,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="16"/>
       <c r="B15" s="17" t="s">
         <v>11</v>
@@ -6008,7 +6009,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="16"/>
       <c r="B16" s="17" t="s">
         <v>12</v>
@@ -6024,7 +6025,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="16"/>
       <c r="B17" s="17" t="s">
         <v>13</v>
@@ -6040,7 +6041,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="16"/>
       <c r="B18" s="17" t="s">
         <v>14</v>
@@ -6056,7 +6057,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="16"/>
       <c r="B19" s="17" t="s">
         <v>15</v>
@@ -6072,7 +6073,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="16"/>
       <c r="B20" s="17" t="s">
         <v>16</v>
@@ -6088,7 +6089,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="16"/>
       <c r="B21" s="17" t="s">
         <v>17</v>
@@ -6104,7 +6105,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="16"/>
       <c r="B22" s="17" t="s">
         <v>18</v>
@@ -6120,7 +6121,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="16"/>
       <c r="B23" s="17" t="s">
         <v>19</v>
@@ -6136,7 +6137,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="16"/>
       <c r="B24" s="17" t="s">
         <v>20</v>
@@ -6152,7 +6153,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="16"/>
       <c r="B25" s="17" t="s">
         <v>21</v>
@@ -6168,7 +6169,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
         <v>22</v>
       </c>
@@ -6180,7 +6181,7 @@
         <v>2.3111111111111113</v>
       </c>
     </row>
-    <row r="27" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="16"/>
       <c r="B27" s="17" t="s">
         <v>23</v>
@@ -6196,7 +6197,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="16"/>
       <c r="B28" s="17" t="s">
         <v>24</v>
@@ -6212,7 +6213,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="16"/>
       <c r="B29" s="17" t="s">
         <v>25</v>
@@ -6228,7 +6229,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="16"/>
       <c r="B30" s="17" t="s">
         <v>26</v>
@@ -6244,7 +6245,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="16"/>
       <c r="B31" s="17" t="s">
         <v>27</v>
@@ -6260,7 +6261,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="16"/>
       <c r="B32" s="17" t="s">
         <v>28</v>
@@ -6276,7 +6277,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="21"/>
       <c r="B33" s="22" t="s">
         <v>29</v>
@@ -6292,25 +6293,25 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="H34" s="4"/>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>44</v>
       </c>
@@ -6328,19 +6329,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BF805FA-A023-4EE6-8056-C3DF8591EEA1}">
   <dimension ref="A1:K33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="R15" sqref="R15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="12.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.88671875" customWidth="1"/>
-    <col min="4" max="4" width="14.5546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.85546875" customWidth="1"/>
+    <col min="4" max="4" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A1" s="36" t="s">
         <v>0</v>
       </c>
@@ -6361,7 +6362,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>1</v>
       </c>
@@ -6374,7 +6375,7 @@
         <v>4.1152623344847195</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="16"/>
       <c r="B3" s="17" t="s">
         <v>4</v>
@@ -6400,7 +6401,7 @@
         <v>4.9243450282518708</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="16"/>
       <c r="B4" s="17" t="s">
         <v>5</v>
@@ -6426,7 +6427,7 @@
         <v>3.884536410589039</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="16"/>
       <c r="B5" s="17" t="s">
         <v>3</v>
@@ -6452,7 +6453,7 @@
         <v>14.116311037775247</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="16"/>
       <c r="B6" s="17" t="s">
         <v>6</v>
@@ -6478,7 +6479,7 @@
         <v>2.2525759032821293</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="16"/>
       <c r="B7" s="17" t="s">
         <v>2</v>
@@ -6504,7 +6505,7 @@
         <v>0.11489763977216218</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="16"/>
       <c r="B8" s="20" t="s">
         <v>37</v>
@@ -6517,7 +6518,7 @@
         <v>0.93908151043690491</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="16"/>
       <c r="B9" s="20" t="s">
         <v>38</v>
@@ -6530,7 +6531,7 @@
         <v>14.961310344210933</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="16"/>
       <c r="B10" s="20" t="s">
         <v>39</v>
@@ -6543,7 +6544,7 @@
         <v>2.7226321595552849</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>7</v>
       </c>
@@ -6556,7 +6557,7 @@
         <v>0.33700788447451974</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="16"/>
       <c r="B12" s="17" t="s">
         <v>8</v>
@@ -6582,7 +6583,7 @@
         <v>1.1726060692474833</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="16"/>
       <c r="B13" s="17" t="s">
         <v>9</v>
@@ -6608,7 +6609,7 @@
         <v>0.16164294256230263</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="16"/>
       <c r="B14" s="17" t="s">
         <v>10</v>
@@ -6634,7 +6635,7 @@
         <v>0.73549572187912404</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="16"/>
       <c r="B15" s="17" t="s">
         <v>11</v>
@@ -6649,7 +6650,7 @@
         <v>0.88739157748459541</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="16"/>
       <c r="B16" s="17" t="s">
         <v>12</v>
@@ -6664,7 +6665,7 @@
         <v>3.408850161558914</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="16"/>
       <c r="B17" s="17" t="s">
         <v>13</v>
@@ -6690,7 +6691,7 @@
         <v>1.7330286243519006</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="16"/>
       <c r="B18" s="17" t="s">
         <v>14</v>
@@ -6716,7 +6717,7 @@
         <v>0.96530632991098708</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="16"/>
       <c r="B19" s="17" t="s">
         <v>15</v>
@@ -6742,7 +6743,7 @@
         <v>3.2577488295699566</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="16"/>
       <c r="B20" s="17" t="s">
         <v>16</v>
@@ -6768,7 +6769,7 @@
         <v>33.221816911272064</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="16"/>
       <c r="B21" s="17" t="s">
         <v>17</v>
@@ -6794,7 +6795,7 @@
         <v>0.15828667278936953</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="16"/>
       <c r="B22" s="17" t="s">
         <v>18</v>
@@ -6820,7 +6821,7 @@
         <v>0.5961266780292841</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="16"/>
       <c r="B23" s="17" t="s">
         <v>19</v>
@@ -6846,7 +6847,7 @@
         <v>3.8152565930812243</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="16"/>
       <c r="B24" s="17" t="s">
         <v>20</v>
@@ -6872,7 +6873,7 @@
         <v>1.5184826354299854</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="16"/>
       <c r="B25" s="17" t="s">
         <v>21</v>
@@ -6892,14 +6893,14 @@
         <v>0.96530632991098708</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
         <v>22</v>
       </c>
       <c r="B26" s="19"/>
       <c r="D26" s="9"/>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="16"/>
       <c r="B27" s="17" t="s">
         <v>23</v>
@@ -6919,7 +6920,7 @@
         <v>3.2577488295699566</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="16"/>
       <c r="B28" s="17" t="s">
         <v>24</v>
@@ -6939,7 +6940,7 @@
         <v>33.221816911272064</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="16"/>
       <c r="B29" s="17" t="s">
         <v>25</v>
@@ -6959,7 +6960,7 @@
         <v>0.15828667278936953</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="16"/>
       <c r="B30" s="17" t="s">
         <v>26</v>
@@ -6979,7 +6980,7 @@
         <v>0.5961266780292841</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="16"/>
       <c r="B31" s="17" t="s">
         <v>27</v>
@@ -6999,7 +7000,7 @@
         <v>3.8152565930812243</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="16"/>
       <c r="B32" s="17" t="s">
         <v>28</v>
@@ -7011,7 +7012,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="21"/>
       <c r="B33" s="22" t="s">
         <v>29</v>
@@ -7048,13 +7049,13 @@
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="14.109375"/>
-    <col min="3" max="4" width="28.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="14.140625"/>
+    <col min="3" max="4" width="28.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A1" s="36" t="s">
         <v>0</v>
       </c>
@@ -7066,7 +7067,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
         <v>42</v>
       </c>
@@ -7080,7 +7081,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>1</v>
       </c>
@@ -7088,7 +7089,7 @@
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="16"/>
       <c r="B4" s="17" t="s">
         <v>4</v>
@@ -7096,7 +7097,7 @@
       <c r="C4" s="7"/>
       <c r="D4" s="7"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="16"/>
       <c r="B5" s="17" t="s">
         <v>5</v>
@@ -7104,7 +7105,7 @@
       <c r="C5" s="7"/>
       <c r="D5" s="7"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="16"/>
       <c r="B6" s="17" t="s">
         <v>3</v>
@@ -7118,7 +7119,7 @@
         <v>82.666666666666671</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="16"/>
       <c r="B7" s="17" t="s">
         <v>6</v>
@@ -7126,7 +7127,7 @@
       <c r="C7" s="7"/>
       <c r="D7" s="7"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="16"/>
       <c r="B8" s="17" t="s">
         <v>2</v>
@@ -7134,7 +7135,7 @@
       <c r="C8" s="7"/>
       <c r="D8" s="7"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="16"/>
       <c r="B9" s="20" t="s">
         <v>37</v>
@@ -7142,7 +7143,7 @@
       <c r="C9" s="7"/>
       <c r="D9" s="7"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="16"/>
       <c r="B10" s="20" t="s">
         <v>38</v>
@@ -7150,7 +7151,7 @@
       <c r="C10" s="7"/>
       <c r="D10" s="7"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="16"/>
       <c r="B11" s="20" t="s">
         <v>39</v>
@@ -7158,7 +7159,7 @@
       <c r="C11" s="7"/>
       <c r="D11" s="7"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>7</v>
       </c>
@@ -7171,7 +7172,7 @@
         <v>4.6222222222222227</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="16"/>
       <c r="B13" s="17" t="s">
         <v>8</v>
@@ -7179,7 +7180,7 @@
       <c r="C13" s="7"/>
       <c r="D13" s="7"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="16"/>
       <c r="B14" s="17" t="s">
         <v>9</v>
@@ -7187,7 +7188,7 @@
       <c r="C14" s="7"/>
       <c r="D14" s="7"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="16"/>
       <c r="B15" s="17" t="s">
         <v>10</v>
@@ -7195,7 +7196,7 @@
       <c r="C15" s="7"/>
       <c r="D15" s="7"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="16"/>
       <c r="B16" s="17" t="s">
         <v>11</v>
@@ -7203,7 +7204,7 @@
       <c r="C16" s="7"/>
       <c r="D16" s="7"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="16"/>
       <c r="B17" s="17" t="s">
         <v>12</v>
@@ -7211,7 +7212,7 @@
       <c r="C17" s="7"/>
       <c r="D17" s="7"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="16"/>
       <c r="B18" s="17" t="s">
         <v>13</v>
@@ -7219,7 +7220,7 @@
       <c r="C18" s="7"/>
       <c r="D18" s="7"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="16"/>
       <c r="B19" s="17" t="s">
         <v>14</v>
@@ -7227,7 +7228,7 @@
       <c r="C19" s="7"/>
       <c r="D19" s="7"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="16"/>
       <c r="B20" s="17" t="s">
         <v>15</v>
@@ -7235,7 +7236,7 @@
       <c r="C20" s="7"/>
       <c r="D20" s="7"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="16"/>
       <c r="B21" s="17" t="s">
         <v>16</v>
@@ -7243,7 +7244,7 @@
       <c r="C21" s="7"/>
       <c r="D21" s="7"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="16"/>
       <c r="B22" s="17" t="s">
         <v>17</v>
@@ -7251,7 +7252,7 @@
       <c r="C22" s="7"/>
       <c r="D22" s="7"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="16"/>
       <c r="B23" s="17" t="s">
         <v>18</v>
@@ -7259,7 +7260,7 @@
       <c r="C23" s="7"/>
       <c r="D23" s="7"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="16"/>
       <c r="B24" s="17" t="s">
         <v>19</v>
@@ -7267,7 +7268,7 @@
       <c r="C24" s="7"/>
       <c r="D24" s="7"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="16"/>
       <c r="B25" s="17" t="s">
         <v>20</v>
@@ -7275,7 +7276,7 @@
       <c r="C25" s="7"/>
       <c r="D25" s="7"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="16"/>
       <c r="B26" s="17" t="s">
         <v>21</v>
@@ -7283,7 +7284,7 @@
       <c r="C26" s="7"/>
       <c r="D26" s="7"/>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
         <v>22</v>
       </c>
@@ -7297,7 +7298,7 @@
         <v>2.3111111111111113</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="16"/>
       <c r="B28" s="17" t="s">
         <v>23</v>
@@ -7305,7 +7306,7 @@
       <c r="C28" s="7"/>
       <c r="D28" s="7"/>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="16"/>
       <c r="B29" s="17" t="s">
         <v>24</v>
@@ -7313,7 +7314,7 @@
       <c r="C29" s="7"/>
       <c r="D29" s="7"/>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="16"/>
       <c r="B30" s="17" t="s">
         <v>25</v>
@@ -7321,7 +7322,7 @@
       <c r="C30" s="7"/>
       <c r="D30" s="7"/>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="16"/>
       <c r="B31" s="17" t="s">
         <v>26</v>
@@ -7329,7 +7330,7 @@
       <c r="C31" s="7"/>
       <c r="D31" s="7"/>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="16"/>
       <c r="B32" s="17" t="s">
         <v>27</v>
@@ -7337,7 +7338,7 @@
       <c r="C32" s="7"/>
       <c r="D32" s="7"/>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="16"/>
       <c r="B33" s="17" t="s">
         <v>28</v>
@@ -7345,7 +7346,7 @@
       <c r="C33" s="7"/>
       <c r="D33" s="7"/>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="21"/>
       <c r="B34" s="22" t="s">
         <v>29</v>
@@ -7353,22 +7354,22 @@
       <c r="C34" s="10"/>
       <c r="D34" s="10"/>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>44</v>
       </c>
@@ -7389,13 +7390,13 @@
       <selection activeCell="T81" sqref="A64:T81"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>60</v>
       </c>
@@ -7410,7 +7411,7 @@
       <c r="J1" s="10"/>
       <c r="K1" s="10"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="24"/>
       <c r="B2" s="27"/>
       <c r="C2" s="41" t="s">
@@ -7425,7 +7426,7 @@
       <c r="J2" s="42"/>
       <c r="K2" s="42"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="34" t="s">
         <v>47</v>
       </c>
@@ -7460,7 +7461,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="33" t="s">
         <v>59</v>
       </c>
@@ -7495,7 +7496,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="34" t="s">
         <v>61</v>
       </c>
@@ -7530,7 +7531,7 @@
         <v>1.6</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="34" t="s">
         <v>62</v>
       </c>
@@ -7565,7 +7566,7 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="34" t="s">
         <v>63</v>
       </c>
@@ -7600,7 +7601,7 @@
         <v>1.8</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="34" t="s">
         <v>64</v>
       </c>
@@ -7635,7 +7636,7 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="34" t="s">
         <v>65</v>
       </c>
@@ -7670,7 +7671,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="34" t="s">
         <v>66</v>
       </c>
@@ -7705,7 +7706,7 @@
         <v>2.4</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="34" t="s">
         <v>67</v>
       </c>
@@ -7740,7 +7741,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="34" t="s">
         <v>68</v>
       </c>
@@ -7775,7 +7776,7 @@
         <v>1.4</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="34" t="s">
         <v>69</v>
       </c>
@@ -7810,7 +7811,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="34" t="s">
         <v>70</v>
       </c>
@@ -7845,7 +7846,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="34" t="s">
         <v>71</v>
       </c>
@@ -7880,7 +7881,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="34" t="s">
         <v>72</v>
       </c>
@@ -7915,7 +7916,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="34" t="s">
         <v>73</v>
       </c>
@@ -7950,7 +7951,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="34" t="s">
         <v>74</v>
       </c>
@@ -7985,7 +7986,7 @@
         <v>1.4</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="25" t="s">
         <v>75</v>
       </c>
@@ -8020,12 +8021,12 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="26"/>
       <c r="B22" s="4"/>
       <c r="C22" s="40" t="s">
@@ -8040,7 +8041,7 @@
       <c r="J22" s="40"/>
       <c r="K22" s="40"/>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="23" t="s">
         <v>47</v>
       </c>
@@ -8075,7 +8076,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="33" t="s">
         <v>59</v>
       </c>
@@ -8110,7 +8111,7 @@
         <v>2.4</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="34" t="s">
         <v>61</v>
       </c>
@@ -8145,7 +8146,7 @@
         <v>2.7</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="34" t="s">
         <v>62</v>
       </c>
@@ -8180,7 +8181,7 @@
         <v>3.3</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="34" t="s">
         <v>63</v>
       </c>
@@ -8215,7 +8216,7 @@
         <v>2.2000000000000002</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="34" t="s">
         <v>64</v>
       </c>
@@ -8250,7 +8251,7 @@
         <v>1.8</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="34" t="s">
         <v>65</v>
       </c>
@@ -8285,7 +8286,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="34" t="s">
         <v>66</v>
       </c>
@@ -8320,7 +8321,7 @@
         <v>1.4</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="34" t="s">
         <v>67</v>
       </c>
@@ -8355,7 +8356,7 @@
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="34" t="s">
         <v>68</v>
       </c>
@@ -8390,7 +8391,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A33" s="34" t="s">
         <v>69</v>
       </c>
@@ -8425,7 +8426,7 @@
         <v>3.1</v>
       </c>
     </row>
-    <row r="34" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A34" s="34" t="s">
         <v>70</v>
       </c>
@@ -8460,7 +8461,7 @@
         <v>2.2000000000000002</v>
       </c>
     </row>
-    <row r="35" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A35" s="34" t="s">
         <v>71</v>
       </c>
@@ -8495,7 +8496,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="36" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A36" s="34" t="s">
         <v>72</v>
       </c>
@@ -8530,7 +8531,7 @@
         <v>2.8</v>
       </c>
     </row>
-    <row r="37" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A37" s="34" t="s">
         <v>73</v>
       </c>
@@ -8565,7 +8566,7 @@
         <v>2.7</v>
       </c>
     </row>
-    <row r="38" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A38" s="34" t="s">
         <v>74</v>
       </c>
@@ -8600,7 +8601,7 @@
         <v>1.9</v>
       </c>
     </row>
-    <row r="39" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A39" s="25" t="s">
         <v>75</v>
       </c>
@@ -8635,7 +8636,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A43" s="24"/>
       <c r="B43" s="27"/>
       <c r="C43" s="43" t="s">
@@ -8662,7 +8663,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="44" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A44" s="34" t="s">
         <v>47</v>
       </c>
@@ -8724,7 +8725,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="45" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A45" s="33" t="s">
         <v>59</v>
       </c>
@@ -8790,7 +8791,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="46" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A46" s="34" t="s">
         <v>61</v>
       </c>
@@ -8856,7 +8857,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="47" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A47" s="34" t="s">
         <v>62</v>
       </c>
@@ -8922,7 +8923,7 @@
         <v>770</v>
       </c>
     </row>
-    <row r="48" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A48" s="34" t="s">
         <v>63</v>
       </c>
@@ -8988,7 +8989,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="49" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A49" s="34" t="s">
         <v>64</v>
       </c>
@@ -9054,7 +9055,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="50" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A50" s="34" t="s">
         <v>65</v>
       </c>
@@ -9120,7 +9121,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="51" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A51" s="34" t="s">
         <v>66</v>
       </c>
@@ -9186,7 +9187,7 @@
         <v>890</v>
       </c>
     </row>
-    <row r="52" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A52" s="34" t="s">
         <v>67</v>
       </c>
@@ -9252,7 +9253,7 @@
         <v>490.00000000000006</v>
       </c>
     </row>
-    <row r="53" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A53" s="34" t="s">
         <v>68</v>
       </c>
@@ -9318,7 +9319,7 @@
         <v>229.99999999999997</v>
       </c>
     </row>
-    <row r="54" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A54" s="34" t="s">
         <v>69</v>
       </c>
@@ -9384,7 +9385,7 @@
         <v>459.99999999999994</v>
       </c>
     </row>
-    <row r="55" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A55" s="34" t="s">
         <v>70</v>
       </c>
@@ -9450,7 +9451,7 @@
         <v>220.00000000000003</v>
       </c>
     </row>
-    <row r="56" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A56" s="34" t="s">
         <v>71</v>
       </c>
@@ -9516,7 +9517,7 @@
         <v>110.00000000000001</v>
       </c>
     </row>
-    <row r="57" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A57" s="34" t="s">
         <v>72</v>
       </c>
@@ -9582,7 +9583,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="58" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A58" s="34" t="s">
         <v>73</v>
       </c>
@@ -9648,7 +9649,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="59" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A59" s="34" t="s">
         <v>74</v>
       </c>
@@ -9714,7 +9715,7 @@
         <v>969.99999999999989</v>
       </c>
     </row>
-    <row r="60" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A60" s="25" t="s">
         <v>75</v>
       </c>
@@ -9780,7 +9781,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="64" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A64" s="24"/>
       <c r="B64" s="38" t="s">
         <v>90</v>
@@ -9804,7 +9805,7 @@
       <c r="S64" s="38"/>
       <c r="T64" s="39"/>
     </row>
-    <row r="65" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A65" s="34" t="s">
         <v>47</v>
       </c>
@@ -9866,7 +9867,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="66" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A66" s="26" t="s">
         <v>59</v>
       </c>
@@ -9947,7 +9948,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="67" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A67" s="29" t="s">
         <v>61</v>
       </c>
@@ -10028,7 +10029,7 @@
         <v>1.0384615384615385</v>
       </c>
     </row>
-    <row r="68" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A68" s="29" t="s">
         <v>62</v>
       </c>
@@ -10109,7 +10110,7 @@
         <v>0.42857142857142855</v>
       </c>
     </row>
-    <row r="69" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A69" s="29" t="s">
         <v>63</v>
       </c>
@@ -10190,7 +10191,7 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="70" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A70" s="29" t="s">
         <v>64</v>
       </c>
@@ -10271,7 +10272,7 @@
         <v>0.29032258064516131</v>
       </c>
     </row>
-    <row r="71" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A71" s="29" t="s">
         <v>65</v>
       </c>
@@ -10352,7 +10353,7 @@
         <v>0.46511627906976744</v>
       </c>
     </row>
-    <row r="72" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A72" s="29" t="s">
         <v>66</v>
       </c>
@@ -10433,7 +10434,7 @@
         <v>0.15730337078651685</v>
       </c>
     </row>
-    <row r="73" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A73" s="29" t="s">
         <v>67</v>
       </c>
@@ -10514,7 +10515,7 @@
         <v>0.46938775510204073</v>
       </c>
     </row>
-    <row r="74" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A74" s="29" t="s">
         <v>68</v>
       </c>
@@ -10595,7 +10596,7 @@
         <v>0.86956521739130443</v>
       </c>
     </row>
-    <row r="75" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A75" s="29" t="s">
         <v>69</v>
       </c>
@@ -10676,7 +10677,7 @@
         <v>0.67391304347826098</v>
       </c>
     </row>
-    <row r="76" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A76" s="29" t="s">
         <v>70</v>
       </c>
@@ -10757,7 +10758,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A77" s="29" t="s">
         <v>71</v>
       </c>
@@ -10838,7 +10839,7 @@
         <v>0.81818181818181812</v>
       </c>
     </row>
-    <row r="78" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A78" s="29" t="s">
         <v>72</v>
       </c>
@@ -10919,7 +10920,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="79" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A79" s="29" t="s">
         <v>73</v>
       </c>
@@ -11000,7 +11001,7 @@
         <v>0.67500000000000004</v>
       </c>
     </row>
-    <row r="80" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A80" s="29" t="s">
         <v>74</v>
       </c>
@@ -11081,7 +11082,7 @@
         <v>0.19587628865979384</v>
       </c>
     </row>
-    <row r="81" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A81" s="31" t="s">
         <v>75</v>
       </c>
@@ -11162,7 +11163,7 @@
         <v>0.47619047619047616</v>
       </c>
     </row>
-    <row r="85" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A85" s="35" t="s">
         <v>91</v>
       </c>
@@ -11184,16 +11185,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2844DBCD-562A-4DC9-AC18-88D586A00EB2}">
   <dimension ref="A1:T42"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="T42" sqref="A26:T42"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="G46" sqref="G46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -11246,7 +11247,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>92</v>
       </c>
@@ -11299,7 +11300,7 @@
         <v>52.380952380952387</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>93</v>
       </c>
@@ -11352,7 +11353,7 @@
         <v>1.4285714285714286</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>94</v>
       </c>
@@ -11405,7 +11406,7 @@
         <v>0.2857142857142857</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>95</v>
       </c>
@@ -11458,7 +11459,7 @@
         <v>32.714285714285715</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>96</v>
       </c>
@@ -11511,7 +11512,7 @@
         <v>1.6190476190476191</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>98</v>
       </c>
@@ -11564,7 +11565,7 @@
         <v>1.7619047619047619</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>97</v>
       </c>
@@ -11617,7 +11618,7 @@
         <v>3.1904761904761907</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>99</v>
       </c>
@@ -11670,7 +11671,7 @@
         <v>0.38095238095238093</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>100</v>
       </c>
@@ -11723,7 +11724,7 @@
         <v>2.0952380952380953</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>101</v>
       </c>
@@ -11776,7 +11777,7 @@
         <v>0.23809523809523808</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>102</v>
       </c>
@@ -11829,7 +11830,7 @@
         <v>1.5714285714285714</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>103</v>
       </c>
@@ -11882,7 +11883,7 @@
         <v>0.23809523809523808</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>104</v>
       </c>
@@ -11935,7 +11936,7 @@
         <v>0.2857142857142857</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>105</v>
       </c>
@@ -11988,7 +11989,7 @@
         <v>0.47619047619047616</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>106</v>
       </c>
@@ -12041,7 +12042,7 @@
         <v>9.5238095238095233E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>107</v>
       </c>
@@ -12094,7 +12095,7 @@
         <v>0.19047619047619047</v>
       </c>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>108</v>
       </c>
@@ -12147,7 +12148,7 @@
         <v>0.47619047619047616</v>
       </c>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>109</v>
       </c>
@@ -12200,7 +12201,7 @@
         <v>9.5238095238095233E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>110</v>
       </c>
@@ -12253,7 +12254,7 @@
         <v>0.47619047619047616</v>
       </c>
     </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B25" s="44" t="s">
         <v>90</v>
       </c>
@@ -12276,7 +12277,7 @@
       <c r="S25" s="44"/>
       <c r="T25" s="44"/>
     </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>47</v>
       </c>
@@ -12338,7 +12339,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>59</v>
       </c>
@@ -12419,7 +12420,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>61</v>
       </c>
@@ -12500,7 +12501,7 @@
         <v>1.04</v>
       </c>
     </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>62</v>
       </c>
@@ -12581,7 +12582,7 @@
         <v>0.43</v>
       </c>
     </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>63</v>
       </c>
@@ -12662,7 +12663,7 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>64</v>
       </c>
@@ -12743,7 +12744,7 @@
         <v>0.28999999999999998</v>
       </c>
     </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>65</v>
       </c>
@@ -12824,7 +12825,7 @@
         <v>0.47</v>
       </c>
     </row>
-    <row r="33" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>66</v>
       </c>
@@ -12905,7 +12906,7 @@
         <v>0.16</v>
       </c>
     </row>
-    <row r="34" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>67</v>
       </c>
@@ -12986,7 +12987,7 @@
         <v>0.47</v>
       </c>
     </row>
-    <row r="35" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>68</v>
       </c>
@@ -13067,7 +13068,7 @@
         <v>0.87</v>
       </c>
     </row>
-    <row r="36" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>69</v>
       </c>
@@ -13148,7 +13149,7 @@
         <v>0.67</v>
       </c>
     </row>
-    <row r="37" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>70</v>
       </c>
@@ -13229,7 +13230,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>71</v>
       </c>
@@ -13310,7 +13311,7 @@
         <v>0.82</v>
       </c>
     </row>
-    <row r="39" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>72</v>
       </c>
@@ -13391,7 +13392,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>73</v>
       </c>
@@ -13472,7 +13473,7 @@
         <v>0.68</v>
       </c>
     </row>
-    <row r="41" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>74</v>
       </c>
@@ -13553,7 +13554,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="42" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>75</v>
       </c>
@@ -13644,6 +13645,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100453E70DD9CB01644826790A9CAD4F8E5" ma:contentTypeVersion="8" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="4194a16a9ad153fca84f039f8f87f351">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="12da1371-c0bd-46af-a584-d0ca56511368" xmlns:ns4="cb9691b9-6864-4b4e-9d45-a7fab6b1f025" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9a9013baf4d91fb8d7883227178a33f6" ns3:_="" ns4:_="">
     <xsd:import namespace="12da1371-c0bd-46af-a584-d0ca56511368"/>
@@ -13834,36 +13850,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BFD9B328-3ECF-4D39-B724-4004F8BBF645}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2C2E367E-E9DE-4053-B8D0-2C7592B152DB}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="12da1371-c0bd-46af-a584-d0ca56511368"/>
-    <ds:schemaRef ds:uri="cb9691b9-6864-4b4e-9d45-a7fab6b1f025"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -13886,9 +13876,20 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2C2E367E-E9DE-4053-B8D0-2C7592B152DB}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BFD9B328-3ECF-4D39-B724-4004F8BBF645}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="12da1371-c0bd-46af-a584-d0ca56511368"/>
+    <ds:schemaRef ds:uri="cb9691b9-6864-4b4e-9d45-a7fab6b1f025"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>